<commit_message>
add condition specificity info to cluster supplementary table
</commit_message>
<xml_diff>
--- a/src/6_functional_interaction/results/clustering_nde75ntotal50_enrichment_annotated.xlsx
+++ b/src/6_functional_interaction/results/clustering_nde75ntotal50_enrichment_annotated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rzhu/Gladstone Dropbox/Ronghui Zhu/GRNPerturbSeq/4_codes/GWT_perturbseq_analysis/src/6_functional_interaction/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939B8B9D-8B2B-7D41-A564-3EE44CF080C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453A3E7B-F4D4-DA43-9DAC-513DC771E9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{AE44F2CC-892D-F147-8D31-099354A290F9}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1504" uniqueCount="769">
   <si>
     <t>cluster</t>
   </si>
@@ -2297,6 +2297,39 @@
   </si>
   <si>
     <t>genome defense</t>
+  </si>
+  <si>
+    <t>corr_rest</t>
+  </si>
+  <si>
+    <t>corr_stim8hr</t>
+  </si>
+  <si>
+    <t>corr_stim48hr</t>
+  </si>
+  <si>
+    <t>corr_shared</t>
+  </si>
+  <si>
+    <t>condition_specificity</t>
+  </si>
+  <si>
+    <t>across_condition</t>
+  </si>
+  <si>
+    <t>Stim8hr</t>
+  </si>
+  <si>
+    <t>Stim8hr_Stim48hr</t>
+  </si>
+  <si>
+    <t>Rest</t>
+  </si>
+  <si>
+    <t>Stim48hr</t>
+  </si>
+  <si>
+    <t>Rest_Stim8hr</t>
   </si>
 </sst>
 </file>
@@ -3138,12 +3171,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA81DAE6-2760-9145-ACBD-851BF9FC920B}">
-  <dimension ref="A1:AQ113"/>
+  <dimension ref="A1:AV113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A46" sqref="A46"/>
-      <selection pane="topRight" activeCell="H8" sqref="H8"/>
+      <selection pane="topRight" activeCell="AR1" sqref="AR1:AV1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3170,7 +3203,7 @@
     <col min="39" max="39" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3300,8 +3333,23 @@
       <c r="AQ1" t="s">
         <v>645</v>
       </c>
+      <c r="AR1" t="s">
+        <v>758</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>759</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>760</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>761</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>762</v>
+      </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3431,8 +3479,23 @@
       <c r="AQ2">
         <v>1</v>
       </c>
+      <c r="AR2">
+        <v>0.40648157264866502</v>
+      </c>
+      <c r="AS2">
+        <v>0.51297608215929202</v>
+      </c>
+      <c r="AT2">
+        <v>0.49674284784620598</v>
+      </c>
+      <c r="AU2">
+        <v>0.35607590946914303</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3562,8 +3625,23 @@
       <c r="AQ3">
         <v>1</v>
       </c>
+      <c r="AR3">
+        <v>0.38271143951381198</v>
+      </c>
+      <c r="AS3">
+        <v>0.41156398933175597</v>
+      </c>
+      <c r="AT3">
+        <v>0.29206693582232202</v>
+      </c>
+      <c r="AU3">
+        <v>0.327720702663717</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3693,8 +3771,23 @@
       <c r="AQ4" s="1">
         <v>5.5624291777094796E-6</v>
       </c>
+      <c r="AR4">
+        <v>0.26168032925378898</v>
+      </c>
+      <c r="AS4">
+        <v>0.304253618567906</v>
+      </c>
+      <c r="AT4">
+        <v>0.28165853621510001</v>
+      </c>
+      <c r="AU4">
+        <v>0.20715558396926001</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3824,8 +3917,23 @@
       <c r="AQ5">
         <v>1</v>
       </c>
+      <c r="AR5">
+        <v>0.50855539183175003</v>
+      </c>
+      <c r="AS5">
+        <v>0.50356974752498596</v>
+      </c>
+      <c r="AT5">
+        <v>0.45303808566172399</v>
+      </c>
+      <c r="AU5">
+        <v>0.29677971906460099</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3955,8 +4063,23 @@
       <c r="AQ6">
         <v>1</v>
       </c>
+      <c r="AR6">
+        <v>0.49469050661269798</v>
+      </c>
+      <c r="AS6">
+        <v>0.51875399674508804</v>
+      </c>
+      <c r="AT6">
+        <v>0.53517958449020597</v>
+      </c>
+      <c r="AU6">
+        <v>0.37651358885085501</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4086,8 +4209,23 @@
       <c r="AQ7">
         <v>1</v>
       </c>
+      <c r="AR7">
+        <v>0.58384714986211395</v>
+      </c>
+      <c r="AS7">
+        <v>0.59607816794851798</v>
+      </c>
+      <c r="AT7">
+        <v>0.59594003507703197</v>
+      </c>
+      <c r="AU7">
+        <v>0.45855450764099598</v>
+      </c>
+      <c r="AV7" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4217,8 +4355,23 @@
       <c r="AQ8">
         <v>1</v>
       </c>
+      <c r="AR8">
+        <v>0.28189776494507501</v>
+      </c>
+      <c r="AS8">
+        <v>0.28429985881269598</v>
+      </c>
+      <c r="AT8">
+        <v>0.20225040592572199</v>
+      </c>
+      <c r="AU8">
+        <v>0.16879182340447499</v>
+      </c>
+      <c r="AV8" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4348,8 +4501,23 @@
       <c r="AQ9">
         <v>1.73975117099044E-3</v>
       </c>
+      <c r="AR9">
+        <v>0.37561466525575599</v>
+      </c>
+      <c r="AS9">
+        <v>0.41273355039861997</v>
+      </c>
+      <c r="AT9">
+        <v>0.25022905039843402</v>
+      </c>
+      <c r="AU9">
+        <v>0.27357749524192898</v>
+      </c>
+      <c r="AV9" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4479,8 +4647,23 @@
       <c r="AQ10" s="1">
         <v>2.0409886145534199E-7</v>
       </c>
+      <c r="AR10">
+        <v>0.287589695131717</v>
+      </c>
+      <c r="AS10">
+        <v>0.34453305238339998</v>
+      </c>
+      <c r="AT10">
+        <v>0.27203185682910003</v>
+      </c>
+      <c r="AU10">
+        <v>0.156596972755804</v>
+      </c>
+      <c r="AV10" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4610,8 +4793,23 @@
       <c r="AQ11">
         <v>1</v>
       </c>
+      <c r="AR11">
+        <v>0.35403665293375902</v>
+      </c>
+      <c r="AS11">
+        <v>0.43224428218294902</v>
+      </c>
+      <c r="AT11">
+        <v>0.37565231970179402</v>
+      </c>
+      <c r="AU11">
+        <v>0.245895864279606</v>
+      </c>
+      <c r="AV11" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4741,8 +4939,23 @@
       <c r="AQ12">
         <v>1</v>
       </c>
+      <c r="AR12">
+        <v>0.311337690331072</v>
+      </c>
+      <c r="AS12">
+        <v>0.40465009802145702</v>
+      </c>
+      <c r="AT12">
+        <v>0.29021946381957803</v>
+      </c>
+      <c r="AU12">
+        <v>0.20646226366123299</v>
+      </c>
+      <c r="AV12" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -4872,8 +5085,23 @@
       <c r="AQ13">
         <v>1</v>
       </c>
+      <c r="AR13">
+        <v>0.75538941529859105</v>
+      </c>
+      <c r="AS13">
+        <v>0.79334963943351999</v>
+      </c>
+      <c r="AT13">
+        <v>0.71902620140918105</v>
+      </c>
+      <c r="AU13">
+        <v>0.451719145779926</v>
+      </c>
+      <c r="AV13" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -5003,8 +5231,23 @@
       <c r="AQ14">
         <v>1</v>
       </c>
+      <c r="AR14">
+        <v>0.24250318930688</v>
+      </c>
+      <c r="AS14">
+        <v>0.34385338412932498</v>
+      </c>
+      <c r="AT14">
+        <v>0.35590591765028901</v>
+      </c>
+      <c r="AU14">
+        <v>0.21874806608835301</v>
+      </c>
+      <c r="AV14" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -5134,8 +5377,23 @@
       <c r="AQ15">
         <v>0.53270693803238101</v>
       </c>
+      <c r="AR15">
+        <v>0.48218023965294599</v>
+      </c>
+      <c r="AS15">
+        <v>0.49235093336580299</v>
+      </c>
+      <c r="AT15">
+        <v>0.34789354864596</v>
+      </c>
+      <c r="AU15">
+        <v>0.30127929243325402</v>
+      </c>
+      <c r="AV15" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -5265,8 +5523,23 @@
       <c r="AQ16">
         <v>1</v>
       </c>
+      <c r="AR16">
+        <v>0.268236380429831</v>
+      </c>
+      <c r="AS16">
+        <v>0.357800520734325</v>
+      </c>
+      <c r="AT16">
+        <v>0.19875531167617599</v>
+      </c>
+      <c r="AU16">
+        <v>0.12201946751661499</v>
+      </c>
+      <c r="AV16" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -5396,8 +5669,23 @@
       <c r="AQ17" s="1">
         <v>1.2946354616844799E-9</v>
       </c>
+      <c r="AR17">
+        <v>0.25503408921506399</v>
+      </c>
+      <c r="AS17">
+        <v>0.37283674663944599</v>
+      </c>
+      <c r="AT17">
+        <v>0.37844895508888199</v>
+      </c>
+      <c r="AU17">
+        <v>0.13771904465812199</v>
+      </c>
+      <c r="AV17" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -5527,8 +5815,23 @@
       <c r="AQ18">
         <v>0.14811624597408399</v>
       </c>
+      <c r="AR18">
+        <v>0.36979401823032998</v>
+      </c>
+      <c r="AS18">
+        <v>0.38330684704201501</v>
+      </c>
+      <c r="AT18">
+        <v>0.38416212936455901</v>
+      </c>
+      <c r="AU18">
+        <v>0.271141655204794</v>
+      </c>
+      <c r="AV18" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -5658,8 +5961,23 @@
       <c r="AQ19">
         <v>1</v>
       </c>
+      <c r="AR19">
+        <v>0.25528761782811898</v>
+      </c>
+      <c r="AS19">
+        <v>0.23844987720317901</v>
+      </c>
+      <c r="AT19">
+        <v>0.26410021817524099</v>
+      </c>
+      <c r="AU19">
+        <v>0.207045604286653</v>
+      </c>
+      <c r="AV19" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -5789,8 +6107,23 @@
       <c r="AQ20">
         <v>1</v>
       </c>
+      <c r="AR20">
+        <v>0.39235980654043201</v>
+      </c>
+      <c r="AS20">
+        <v>0.49322054874429799</v>
+      </c>
+      <c r="AT20">
+        <v>0.55545138138686601</v>
+      </c>
+      <c r="AU20">
+        <v>0.36251967020011999</v>
+      </c>
+      <c r="AV20" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -5920,8 +6253,23 @@
       <c r="AQ21">
         <v>2.8487490568070198E-3</v>
       </c>
+      <c r="AR21">
+        <v>0.20741186107882001</v>
+      </c>
+      <c r="AS21">
+        <v>0.199395605586102</v>
+      </c>
+      <c r="AT21">
+        <v>0.18333538407161301</v>
+      </c>
+      <c r="AU21">
+        <v>0.115186610110244</v>
+      </c>
+      <c r="AV21" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -6051,8 +6399,23 @@
       <c r="AQ22">
         <v>1</v>
       </c>
+      <c r="AR22">
+        <v>0.36252083442198801</v>
+      </c>
+      <c r="AS22">
+        <v>0.27371662107758099</v>
+      </c>
+      <c r="AT22">
+        <v>0.32442984803907698</v>
+      </c>
+      <c r="AU22">
+        <v>0.23232120711534299</v>
+      </c>
+      <c r="AV22" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -6182,8 +6545,23 @@
       <c r="AQ23">
         <v>1</v>
       </c>
+      <c r="AR23">
+        <v>3.3504841932685402E-2</v>
+      </c>
+      <c r="AS23">
+        <v>0.25087596509236298</v>
+      </c>
+      <c r="AT23">
+        <v>0.113018943554052</v>
+      </c>
+      <c r="AU23">
+        <v>7.13760208017446E-2</v>
+      </c>
+      <c r="AV23" t="s">
+        <v>764</v>
+      </c>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -6313,8 +6691,23 @@
       <c r="AQ24" s="1">
         <v>1.06852882848756E-7</v>
       </c>
+      <c r="AR24">
+        <v>0.172067814723216</v>
+      </c>
+      <c r="AS24">
+        <v>0.900215029548178</v>
+      </c>
+      <c r="AT24">
+        <v>0.62014296741337305</v>
+      </c>
+      <c r="AU24">
+        <v>0.29636035489868601</v>
+      </c>
+      <c r="AV24" t="s">
+        <v>765</v>
+      </c>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -6444,8 +6837,23 @@
       <c r="AQ25">
         <v>1</v>
       </c>
+      <c r="AR25">
+        <v>0.28849869005652301</v>
+      </c>
+      <c r="AS25">
+        <v>0.34349970376639899</v>
+      </c>
+      <c r="AT25">
+        <v>0.20409895873579101</v>
+      </c>
+      <c r="AU25">
+        <v>0.17415918154028001</v>
+      </c>
+      <c r="AV25" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -6575,8 +6983,23 @@
       <c r="AQ26">
         <v>0.43477913600627099</v>
       </c>
+      <c r="AR26">
+        <v>0.110588429405108</v>
+      </c>
+      <c r="AS26">
+        <v>0.22876910275840201</v>
+      </c>
+      <c r="AT26">
+        <v>0.11544253539788001</v>
+      </c>
+      <c r="AU26">
+        <v>0.116910295167101</v>
+      </c>
+      <c r="AV26" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -6706,8 +7129,23 @@
       <c r="AQ27">
         <v>1</v>
       </c>
+      <c r="AR27">
+        <v>0.18042577592551301</v>
+      </c>
+      <c r="AS27">
+        <v>7.7102053545282795E-2</v>
+      </c>
+      <c r="AT27">
+        <v>8.0545005470863601E-2</v>
+      </c>
+      <c r="AU27">
+        <v>4.6398651408720799E-2</v>
+      </c>
+      <c r="AV27" t="s">
+        <v>766</v>
+      </c>
     </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -6837,8 +7275,23 @@
       <c r="AQ28">
         <v>1</v>
       </c>
+      <c r="AR28">
+        <v>0.18350073973968201</v>
+      </c>
+      <c r="AS28">
+        <v>3.4000560144319597E-2</v>
+      </c>
+      <c r="AT28">
+        <v>2.4623304586057299E-2</v>
+      </c>
+      <c r="AU28">
+        <v>2.9672100746200601E-2</v>
+      </c>
+      <c r="AV28" t="s">
+        <v>766</v>
+      </c>
     </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -6968,8 +7421,23 @@
       <c r="AQ29">
         <v>1</v>
       </c>
+      <c r="AR29">
+        <v>0.38746167346253202</v>
+      </c>
+      <c r="AS29">
+        <v>8.7457937143009506E-2</v>
+      </c>
+      <c r="AT29">
+        <v>4.3984120189526701E-2</v>
+      </c>
+      <c r="AU29">
+        <v>6.89300535638252E-2</v>
+      </c>
+      <c r="AV29" t="s">
+        <v>766</v>
+      </c>
     </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -7099,8 +7567,23 @@
       <c r="AQ30">
         <v>2.2249771015824E-3</v>
       </c>
+      <c r="AR30">
+        <v>0.29526807576053699</v>
+      </c>
+      <c r="AS30">
+        <v>0.37806008357562898</v>
+      </c>
+      <c r="AT30">
+        <v>0.41565626936480299</v>
+      </c>
+      <c r="AU30">
+        <v>0.15783483621658101</v>
+      </c>
+      <c r="AV30" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -7230,8 +7713,23 @@
       <c r="AQ31">
         <v>1</v>
       </c>
+      <c r="AR31">
+        <v>0.243426488047329</v>
+      </c>
+      <c r="AS31">
+        <v>0.10542800740903099</v>
+      </c>
+      <c r="AT31">
+        <v>8.7875972386729798E-2</v>
+      </c>
+      <c r="AU31">
+        <v>9.1543584829030702E-2</v>
+      </c>
+      <c r="AV31" t="s">
+        <v>766</v>
+      </c>
     </row>
-    <row r="32" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -7361,8 +7859,23 @@
       <c r="AQ32">
         <v>1</v>
       </c>
+      <c r="AR32">
+        <v>0.224973509299247</v>
+      </c>
+      <c r="AS32">
+        <v>0.19122984520759201</v>
+      </c>
+      <c r="AT32">
+        <v>6.63446240441697E-2</v>
+      </c>
+      <c r="AU32">
+        <v>4.77887677872013E-2</v>
+      </c>
+      <c r="AV32" t="s">
+        <v>766</v>
+      </c>
     </row>
-    <row r="33" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
@@ -7492,8 +8005,23 @@
       <c r="AQ33" s="1">
         <v>8.7417697566116596E-8</v>
       </c>
+      <c r="AR33">
+        <v>0.250172878152711</v>
+      </c>
+      <c r="AS33">
+        <v>0.30362092027127802</v>
+      </c>
+      <c r="AT33">
+        <v>0.41401639969723297</v>
+      </c>
+      <c r="AU33">
+        <v>0.17752080633779399</v>
+      </c>
+      <c r="AV33" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="34" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
@@ -7623,8 +8151,23 @@
       <c r="AQ34" s="1">
         <v>2.9806232095459803E-8</v>
       </c>
+      <c r="AR34">
+        <v>0.251501747177026</v>
+      </c>
+      <c r="AS34">
+        <v>0.36115155966906798</v>
+      </c>
+      <c r="AT34">
+        <v>0.372519905534624</v>
+      </c>
+      <c r="AU34">
+        <v>0.191224909942628</v>
+      </c>
+      <c r="AV34" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="35" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
@@ -7754,8 +8297,23 @@
       <c r="AQ35">
         <v>1</v>
       </c>
+      <c r="AR35">
+        <v>0.39622177618814403</v>
+      </c>
+      <c r="AS35">
+        <v>0.42842397973617302</v>
+      </c>
+      <c r="AT35">
+        <v>0.27355318881551799</v>
+      </c>
+      <c r="AU35">
+        <v>0.21671154919640601</v>
+      </c>
+      <c r="AV35" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="36" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
@@ -7885,8 +8443,23 @@
       <c r="AQ36" s="1">
         <v>3.3796601556088003E-5</v>
       </c>
+      <c r="AR36">
+        <v>0.28437150705320302</v>
+      </c>
+      <c r="AS36">
+        <v>0.35165615023746599</v>
+      </c>
+      <c r="AT36">
+        <v>0.27791562295181799</v>
+      </c>
+      <c r="AU36">
+        <v>0.16138126127505301</v>
+      </c>
+      <c r="AV36" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="37" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
@@ -8016,8 +8589,23 @@
       <c r="AQ37">
         <v>1</v>
       </c>
+      <c r="AR37">
+        <v>0.20697038339519999</v>
+      </c>
+      <c r="AS37">
+        <v>0.215302123842608</v>
+      </c>
+      <c r="AT37">
+        <v>0.15472007448007699</v>
+      </c>
+      <c r="AU37">
+        <v>9.7159515932049204E-2</v>
+      </c>
+      <c r="AV37" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="38" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
@@ -8147,8 +8735,23 @@
       <c r="AQ38">
         <v>4.3545347406089303E-3</v>
       </c>
+      <c r="AR38">
+        <v>7.5987417075073102E-2</v>
+      </c>
+      <c r="AS38">
+        <v>8.6317682594838796E-2</v>
+      </c>
+      <c r="AT38">
+        <v>0.39753842683851598</v>
+      </c>
+      <c r="AU38">
+        <v>6.4638964075712096E-2</v>
+      </c>
+      <c r="AV38" t="s">
+        <v>767</v>
+      </c>
     </row>
-    <row r="39" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
@@ -8278,8 +8881,23 @@
       <c r="AQ39">
         <v>1.0773316735043399E-2</v>
       </c>
+      <c r="AR39">
+        <v>0.20352167831267001</v>
+      </c>
+      <c r="AS39">
+        <v>0.29061855031836298</v>
+      </c>
+      <c r="AT39">
+        <v>7.7771240142422704E-2</v>
+      </c>
+      <c r="AU39">
+        <v>0.115547529397677</v>
+      </c>
+      <c r="AV39" t="s">
+        <v>768</v>
+      </c>
     </row>
-    <row r="40" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
@@ -8409,8 +9027,23 @@
       <c r="AQ40">
         <v>1</v>
       </c>
+      <c r="AR40">
+        <v>0.23122864775617699</v>
+      </c>
+      <c r="AS40">
+        <v>0.267279913130827</v>
+      </c>
+      <c r="AT40">
+        <v>0.32149989690660102</v>
+      </c>
+      <c r="AU40">
+        <v>0.16949293678261601</v>
+      </c>
+      <c r="AV40" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="41" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
@@ -8540,8 +9173,23 @@
       <c r="AQ41">
         <v>1</v>
       </c>
+      <c r="AR41">
+        <v>0.134536090906998</v>
+      </c>
+      <c r="AS41">
+        <v>0.14010723758882401</v>
+      </c>
+      <c r="AT41">
+        <v>0.13399534147001699</v>
+      </c>
+      <c r="AU41">
+        <v>9.0479769947255401E-2</v>
+      </c>
+      <c r="AV41" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="42" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
@@ -8671,8 +9319,23 @@
       <c r="AQ42">
         <v>1</v>
       </c>
+      <c r="AR42">
+        <v>0.186772062054714</v>
+      </c>
+      <c r="AS42">
+        <v>0.175079787843753</v>
+      </c>
+      <c r="AT42">
+        <v>0.25768093288912097</v>
+      </c>
+      <c r="AU42">
+        <v>0.12836132264198299</v>
+      </c>
+      <c r="AV42" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="43" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>41</v>
       </c>
@@ -8802,8 +9465,23 @@
       <c r="AQ43">
         <v>2.3810335383512302E-3</v>
       </c>
+      <c r="AR43">
+        <v>0.16152240835103901</v>
+      </c>
+      <c r="AS43">
+        <v>0.20250903713642901</v>
+      </c>
+      <c r="AT43">
+        <v>8.2737605975873804E-2</v>
+      </c>
+      <c r="AU43">
+        <v>0.11389618134115</v>
+      </c>
+      <c r="AV43" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="44" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>42</v>
       </c>
@@ -8933,8 +9611,23 @@
       <c r="AQ44">
         <v>1</v>
       </c>
+      <c r="AR44">
+        <v>0.16674749886375401</v>
+      </c>
+      <c r="AS44">
+        <v>0.13171643414008</v>
+      </c>
+      <c r="AT44">
+        <v>5.6037628746958203E-2</v>
+      </c>
+      <c r="AU44">
+        <v>6.8663211981368794E-2</v>
+      </c>
+      <c r="AV44" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="45" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>43</v>
       </c>
@@ -9064,8 +9757,23 @@
       <c r="AQ45">
         <v>1</v>
       </c>
+      <c r="AR45">
+        <v>0.34845211077336302</v>
+      </c>
+      <c r="AS45">
+        <v>0.37356738862746602</v>
+      </c>
+      <c r="AT45">
+        <v>0.41849434646970501</v>
+      </c>
+      <c r="AU45">
+        <v>0.228452239957908</v>
+      </c>
+      <c r="AV45" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="46" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>44</v>
       </c>
@@ -9195,8 +9903,23 @@
       <c r="AQ46">
         <v>1</v>
       </c>
+      <c r="AR46">
+        <v>0.22972189862016201</v>
+      </c>
+      <c r="AS46">
+        <v>0.27931444905078001</v>
+      </c>
+      <c r="AT46">
+        <v>0.29921232871306602</v>
+      </c>
+      <c r="AU46">
+        <v>0.16489458507812399</v>
+      </c>
+      <c r="AV46" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="47" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>45</v>
       </c>
@@ -9326,8 +10049,23 @@
       <c r="AQ47">
         <v>1</v>
       </c>
+      <c r="AR47">
+        <v>7.8767443366201104E-2</v>
+      </c>
+      <c r="AS47">
+        <v>3.6334667614455897E-2</v>
+      </c>
+      <c r="AT47">
+        <v>3.2501420696840901E-2</v>
+      </c>
+      <c r="AU47">
+        <v>3.8355007838106699E-2</v>
+      </c>
+      <c r="AV47" t="s">
+        <v>766</v>
+      </c>
     </row>
-    <row r="48" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>46</v>
       </c>
@@ -9457,8 +10195,23 @@
       <c r="AQ48">
         <v>1</v>
       </c>
+      <c r="AR48">
+        <v>0.38543682840562299</v>
+      </c>
+      <c r="AS48">
+        <v>0.36959149065069402</v>
+      </c>
+      <c r="AT48">
+        <v>0.24127164564936701</v>
+      </c>
+      <c r="AU48">
+        <v>0.13593278050574401</v>
+      </c>
+      <c r="AV48" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="49" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>47</v>
       </c>
@@ -9588,8 +10341,23 @@
       <c r="AQ49">
         <v>1</v>
       </c>
+      <c r="AR49">
+        <v>0.373931850626191</v>
+      </c>
+      <c r="AS49">
+        <v>0.33861540451188898</v>
+      </c>
+      <c r="AT49">
+        <v>0.32563880836249298</v>
+      </c>
+      <c r="AU49">
+        <v>0.257956346514153</v>
+      </c>
+      <c r="AV49" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="50" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>48</v>
       </c>
@@ -9719,8 +10487,23 @@
       <c r="AQ50">
         <v>1.12388282374984E-2</v>
       </c>
+      <c r="AR50">
+        <v>0.32968273420414701</v>
+      </c>
+      <c r="AS50">
+        <v>0.22887767139457299</v>
+      </c>
+      <c r="AT50">
+        <v>0.30003147425503002</v>
+      </c>
+      <c r="AU50">
+        <v>0.15552176616518101</v>
+      </c>
+      <c r="AV50" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="51" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>49</v>
       </c>
@@ -9850,8 +10633,23 @@
       <c r="AQ51">
         <v>1</v>
       </c>
+      <c r="AR51">
+        <v>0.215605048700966</v>
+      </c>
+      <c r="AS51">
+        <v>3.9337523424069001E-2</v>
+      </c>
+      <c r="AT51">
+        <v>1.25448841308342E-2</v>
+      </c>
+      <c r="AU51">
+        <v>2.83840268812376E-2</v>
+      </c>
+      <c r="AV51" t="s">
+        <v>766</v>
+      </c>
     </row>
-    <row r="52" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>50</v>
       </c>
@@ -9981,8 +10779,23 @@
       <c r="AQ52">
         <v>0.69362154960511502</v>
       </c>
+      <c r="AR52">
+        <v>0.16156134884538101</v>
+      </c>
+      <c r="AS52">
+        <v>0.148261743038378</v>
+      </c>
+      <c r="AT52">
+        <v>0.161162129693531</v>
+      </c>
+      <c r="AU52">
+        <v>5.7857263118178598E-2</v>
+      </c>
+      <c r="AV52" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="53" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>51</v>
       </c>
@@ -10112,8 +10925,23 @@
       <c r="AQ53">
         <v>0.17996031575718199</v>
       </c>
+      <c r="AR53">
+        <v>0.21476975991448699</v>
+      </c>
+      <c r="AS53">
+        <v>0.116426118066072</v>
+      </c>
+      <c r="AT53">
+        <v>0.14942735973636001</v>
+      </c>
+      <c r="AU53">
+        <v>5.6503926523180897E-2</v>
+      </c>
+      <c r="AV53" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="54" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>52</v>
       </c>
@@ -10243,8 +11071,23 @@
       <c r="AQ54">
         <v>1</v>
       </c>
+      <c r="AR54">
+        <v>0.34297196646785399</v>
+      </c>
+      <c r="AS54">
+        <v>0.320333345215705</v>
+      </c>
+      <c r="AT54">
+        <v>0.169974847864198</v>
+      </c>
+      <c r="AU54">
+        <v>0.13967692641989399</v>
+      </c>
+      <c r="AV54" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="55" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>53</v>
       </c>
@@ -10374,8 +11217,23 @@
       <c r="AQ55">
         <v>1</v>
       </c>
+      <c r="AR55">
+        <v>9.1972968582308301E-2</v>
+      </c>
+      <c r="AS55">
+        <v>0.187582977509199</v>
+      </c>
+      <c r="AT55">
+        <v>6.3077173217919003E-2</v>
+      </c>
+      <c r="AU55">
+        <v>5.3531723514045899E-2</v>
+      </c>
+      <c r="AV55" t="s">
+        <v>764</v>
+      </c>
     </row>
-    <row r="56" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>54</v>
       </c>
@@ -10505,8 +11363,23 @@
       <c r="AQ56">
         <v>1</v>
       </c>
+      <c r="AR56">
+        <v>0.25139559160368102</v>
+      </c>
+      <c r="AS56">
+        <v>0.23161495180429401</v>
+      </c>
+      <c r="AT56">
+        <v>5.0932947357760001E-2</v>
+      </c>
+      <c r="AU56">
+        <v>6.2277401798033601E-2</v>
+      </c>
+      <c r="AV56" t="s">
+        <v>768</v>
+      </c>
     </row>
-    <row r="57" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>55</v>
       </c>
@@ -10636,8 +11509,23 @@
       <c r="AQ57">
         <v>1</v>
       </c>
+      <c r="AR57">
+        <v>-4.9630384116220003E-4</v>
+      </c>
+      <c r="AS57">
+        <v>-3.8964381905269498E-2</v>
+      </c>
+      <c r="AT57">
+        <v>1.9475633263060201E-2</v>
+      </c>
+      <c r="AU57">
+        <v>6.983751474702E-4</v>
+      </c>
+      <c r="AV57" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="58" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>56</v>
       </c>
@@ -10767,8 +11655,23 @@
       <c r="AQ58">
         <v>1</v>
       </c>
+      <c r="AR58">
+        <v>0.62813684169987405</v>
+      </c>
+      <c r="AS58">
+        <v>0.50457297407731105</v>
+      </c>
+      <c r="AT58">
+        <v>0.39741083095810298</v>
+      </c>
+      <c r="AU58">
+        <v>0.364886345802932</v>
+      </c>
+      <c r="AV58" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="59" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>57</v>
       </c>
@@ -10898,8 +11801,23 @@
       <c r="AQ59">
         <v>1</v>
       </c>
+      <c r="AR59">
+        <v>7.92065395484782E-2</v>
+      </c>
+      <c r="AS59">
+        <v>6.2758499077573193E-2</v>
+      </c>
+      <c r="AT59">
+        <v>0.31049389368074998</v>
+      </c>
+      <c r="AU59">
+        <v>5.0583446267173898E-2</v>
+      </c>
+      <c r="AV59" t="s">
+        <v>767</v>
+      </c>
     </row>
-    <row r="60" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>58</v>
       </c>
@@ -11029,8 +11947,23 @@
       <c r="AQ60" s="1">
         <v>2.9467520223053903E-20</v>
       </c>
+      <c r="AR60">
+        <v>0.18328800279784399</v>
+      </c>
+      <c r="AS60">
+        <v>0.18756449818594401</v>
+      </c>
+      <c r="AT60">
+        <v>0.37904466656708602</v>
+      </c>
+      <c r="AU60">
+        <v>9.8190380542557701E-2</v>
+      </c>
+      <c r="AV60" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="61" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>59</v>
       </c>
@@ -11160,8 +12093,23 @@
       <c r="AQ61">
         <v>1</v>
       </c>
+      <c r="AR61">
+        <v>0.121364227429205</v>
+      </c>
+      <c r="AS61">
+        <v>0.101895296806969</v>
+      </c>
+      <c r="AT61">
+        <v>0.121308187677632</v>
+      </c>
+      <c r="AU61">
+        <v>7.1749672156205299E-2</v>
+      </c>
+      <c r="AV61" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="62" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>60</v>
       </c>
@@ -11291,8 +12239,23 @@
       <c r="AQ62">
         <v>1</v>
       </c>
+      <c r="AR62">
+        <v>0.24522877116095901</v>
+      </c>
+      <c r="AS62">
+        <v>0.35674486540871603</v>
+      </c>
+      <c r="AT62">
+        <v>9.5396082361758394E-2</v>
+      </c>
+      <c r="AU62">
+        <v>6.0240799549630297E-2</v>
+      </c>
+      <c r="AV62" t="s">
+        <v>768</v>
+      </c>
     </row>
-    <row r="63" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>61</v>
       </c>
@@ -11422,8 +12385,23 @@
       <c r="AQ63">
         <v>1</v>
       </c>
+      <c r="AR63">
+        <v>0.30470667752978903</v>
+      </c>
+      <c r="AS63">
+        <v>0.34105242119623103</v>
+      </c>
+      <c r="AT63">
+        <v>0.19697008382799999</v>
+      </c>
+      <c r="AU63">
+        <v>0.13069833122553401</v>
+      </c>
+      <c r="AV63" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="64" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>62</v>
       </c>
@@ -11553,8 +12531,23 @@
       <c r="AQ64">
         <v>1</v>
       </c>
+      <c r="AR64">
+        <v>0.49386386018753398</v>
+      </c>
+      <c r="AS64">
+        <v>0.39485681153025598</v>
+      </c>
+      <c r="AT64">
+        <v>0.29031800265242202</v>
+      </c>
+      <c r="AU64">
+        <v>0.231727445795535</v>
+      </c>
+      <c r="AV64" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="65" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>63</v>
       </c>
@@ -11684,8 +12677,23 @@
       <c r="AQ65">
         <v>1</v>
       </c>
+      <c r="AR65">
+        <v>0.20668499018887199</v>
+      </c>
+      <c r="AS65">
+        <v>0.22906731319409901</v>
+      </c>
+      <c r="AT65">
+        <v>0.27499469118066</v>
+      </c>
+      <c r="AU65">
+        <v>0.14656653254521099</v>
+      </c>
+      <c r="AV65" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="66" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>64</v>
       </c>
@@ -11815,8 +12823,23 @@
       <c r="AQ66">
         <v>1</v>
       </c>
+      <c r="AR66">
+        <v>0.106869146175161</v>
+      </c>
+      <c r="AS66">
+        <v>9.2900217465541904E-2</v>
+      </c>
+      <c r="AT66">
+        <v>0.12820125328458901</v>
+      </c>
+      <c r="AU66">
+        <v>6.0516094803882002E-2</v>
+      </c>
+      <c r="AV66" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="67" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>65</v>
       </c>
@@ -11946,8 +12969,23 @@
       <c r="AQ67">
         <v>1</v>
       </c>
+      <c r="AR67">
+        <v>0.48498985972303099</v>
+      </c>
+      <c r="AS67">
+        <v>0.50273515618515596</v>
+      </c>
+      <c r="AT67">
+        <v>0.47525301388618602</v>
+      </c>
+      <c r="AU67">
+        <v>0.30802403317891403</v>
+      </c>
+      <c r="AV67" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="68" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>66</v>
       </c>
@@ -12077,8 +13115,23 @@
       <c r="AQ68">
         <v>1</v>
       </c>
+      <c r="AR68">
+        <v>0.48498985972303099</v>
+      </c>
+      <c r="AS68">
+        <v>0.50273515618515596</v>
+      </c>
+      <c r="AT68">
+        <v>0.47525301388618602</v>
+      </c>
+      <c r="AU68">
+        <v>0.30802403317891403</v>
+      </c>
+      <c r="AV68" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="69" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>67</v>
       </c>
@@ -12208,8 +13261,23 @@
       <c r="AQ69">
         <v>1</v>
       </c>
+      <c r="AR69">
+        <v>7.7986698352480399E-2</v>
+      </c>
+      <c r="AS69">
+        <v>0.21351360929719199</v>
+      </c>
+      <c r="AT69">
+        <v>3.9737395730011699E-2</v>
+      </c>
+      <c r="AU69">
+        <v>4.6662803949643797E-2</v>
+      </c>
+      <c r="AV69" t="s">
+        <v>764</v>
+      </c>
     </row>
-    <row r="70" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>68</v>
       </c>
@@ -12339,8 +13407,23 @@
       <c r="AQ70" s="1">
         <v>9.0371734530618098E-5</v>
       </c>
+      <c r="AR70">
+        <v>0.20085245145347499</v>
+      </c>
+      <c r="AS70">
+        <v>0.325302403689186</v>
+      </c>
+      <c r="AT70">
+        <v>0.13201608881397101</v>
+      </c>
+      <c r="AU70">
+        <v>0.111923988620486</v>
+      </c>
+      <c r="AV70" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="71" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>69</v>
       </c>
@@ -12470,8 +13553,23 @@
       <c r="AQ71">
         <v>1</v>
       </c>
+      <c r="AR71">
+        <v>7.5905858579455199E-2</v>
+      </c>
+      <c r="AS71">
+        <v>6.2400265196790899E-2</v>
+      </c>
+      <c r="AT71">
+        <v>3.7098317073143101E-2</v>
+      </c>
+      <c r="AU71">
+        <v>3.5659291108160997E-2</v>
+      </c>
+      <c r="AV71" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="72" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>70</v>
       </c>
@@ -12601,8 +13699,23 @@
       <c r="AQ72">
         <v>0.71151503129643301</v>
       </c>
+      <c r="AR72">
+        <v>0.17148867371832199</v>
+      </c>
+      <c r="AS72">
+        <v>0.23497401176868499</v>
+      </c>
+      <c r="AT72">
+        <v>0.151214584771793</v>
+      </c>
+      <c r="AU72">
+        <v>0.13942275295025799</v>
+      </c>
+      <c r="AV72" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="73" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>71</v>
       </c>
@@ -12732,8 +13845,23 @@
       <c r="AQ73">
         <v>1</v>
       </c>
+      <c r="AR73">
+        <v>9.2598439582371794E-2</v>
+      </c>
+      <c r="AS73">
+        <v>0.14195976445227501</v>
+      </c>
+      <c r="AT73">
+        <v>0.13002722105876399</v>
+      </c>
+      <c r="AU73">
+        <v>0.14542747893691599</v>
+      </c>
+      <c r="AV73" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="74" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>72</v>
       </c>
@@ -12863,8 +13991,23 @@
       <c r="AQ74">
         <v>1</v>
       </c>
+      <c r="AR74">
+        <v>0.24820649282461499</v>
+      </c>
+      <c r="AS74">
+        <v>7.50502611665297E-2</v>
+      </c>
+      <c r="AT74">
+        <v>3.4198618483775499E-2</v>
+      </c>
+      <c r="AU74">
+        <v>3.5390860630754202E-2</v>
+      </c>
+      <c r="AV74" t="s">
+        <v>766</v>
+      </c>
     </row>
-    <row r="75" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>73</v>
       </c>
@@ -12994,8 +14137,23 @@
       <c r="AQ75">
         <v>1</v>
       </c>
+      <c r="AR75">
+        <v>4.14951162538763E-2</v>
+      </c>
+      <c r="AS75">
+        <v>7.3945953394869396E-2</v>
+      </c>
+      <c r="AT75">
+        <v>0.103354162453844</v>
+      </c>
+      <c r="AU75">
+        <v>5.3846482451243599E-2</v>
+      </c>
+      <c r="AV75" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="76" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>74</v>
       </c>
@@ -13125,8 +14283,23 @@
       <c r="AQ76">
         <v>1</v>
       </c>
+      <c r="AR76">
+        <v>0.225857347223547</v>
+      </c>
+      <c r="AS76">
+        <v>0.319560876850779</v>
+      </c>
+      <c r="AT76">
+        <v>0.286553898566551</v>
+      </c>
+      <c r="AU76">
+        <v>0.112902830722226</v>
+      </c>
+      <c r="AV76" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="77" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>75</v>
       </c>
@@ -13256,8 +14429,23 @@
       <c r="AQ77">
         <v>1</v>
       </c>
+      <c r="AR77">
+        <v>0.33022771554444202</v>
+      </c>
+      <c r="AS77">
+        <v>0.12308387274312101</v>
+      </c>
+      <c r="AT77">
+        <v>5.7215501257170898E-2</v>
+      </c>
+      <c r="AU77">
+        <v>7.4355333464021095E-2</v>
+      </c>
+      <c r="AV77" t="s">
+        <v>766</v>
+      </c>
     </row>
-    <row r="78" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>76</v>
       </c>
@@ -13387,8 +14575,23 @@
       <c r="AQ78">
         <v>1</v>
       </c>
+      <c r="AR78">
+        <v>3.3634521580691697E-2</v>
+      </c>
+      <c r="AS78">
+        <v>3.7936240309417099E-2</v>
+      </c>
+      <c r="AT78">
+        <v>0.15485081356272401</v>
+      </c>
+      <c r="AU78">
+        <v>2.3850552053401201E-2</v>
+      </c>
+      <c r="AV78" t="s">
+        <v>767</v>
+      </c>
     </row>
-    <row r="79" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>77</v>
       </c>
@@ -13518,8 +14721,23 @@
       <c r="AQ79">
         <v>1</v>
       </c>
+      <c r="AR79">
+        <v>4.4033365616632902E-2</v>
+      </c>
+      <c r="AS79">
+        <v>3.5389745744152698E-2</v>
+      </c>
+      <c r="AT79">
+        <v>0.25573679194922999</v>
+      </c>
+      <c r="AU79">
+        <v>4.1339331645289197E-2</v>
+      </c>
+      <c r="AV79" t="s">
+        <v>767</v>
+      </c>
     </row>
-    <row r="80" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>78</v>
       </c>
@@ -13649,8 +14867,23 @@
       <c r="AQ80">
         <v>1</v>
       </c>
+      <c r="AR80">
+        <v>0.15227071501335401</v>
+      </c>
+      <c r="AS80">
+        <v>0.17200271580357601</v>
+      </c>
+      <c r="AT80">
+        <v>0.27844877914084598</v>
+      </c>
+      <c r="AU80">
+        <v>0.121569601813637</v>
+      </c>
+      <c r="AV80" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="81" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>79</v>
       </c>
@@ -13780,8 +15013,23 @@
       <c r="AQ81">
         <v>0.26340044543177898</v>
       </c>
+      <c r="AR81">
+        <v>0.30491986556016298</v>
+      </c>
+      <c r="AS81">
+        <v>0.21322057865573801</v>
+      </c>
+      <c r="AT81">
+        <v>0.184010658074235</v>
+      </c>
+      <c r="AU81">
+        <v>9.9303900106460397E-2</v>
+      </c>
+      <c r="AV81" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="82" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>80</v>
       </c>
@@ -13911,8 +15159,23 @@
       <c r="AQ82">
         <v>1</v>
       </c>
+      <c r="AR82">
+        <v>0.147428943789184</v>
+      </c>
+      <c r="AS82">
+        <v>0.13566781398655101</v>
+      </c>
+      <c r="AT82">
+        <v>4.3363498081228698E-2</v>
+      </c>
+      <c r="AU82">
+        <v>4.2872357048438899E-2</v>
+      </c>
+      <c r="AV82" t="s">
+        <v>768</v>
+      </c>
     </row>
-    <row r="83" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>81</v>
       </c>
@@ -14042,8 +15305,23 @@
       <c r="AQ83" s="1">
         <v>6.9764843805621097E-5</v>
       </c>
+      <c r="AR83">
+        <v>0.351597677908358</v>
+      </c>
+      <c r="AS83">
+        <v>0.37319360583713501</v>
+      </c>
+      <c r="AT83">
+        <v>0.378375731639229</v>
+      </c>
+      <c r="AU83">
+        <v>0.27571699939382699</v>
+      </c>
+      <c r="AV83" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="84" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>82</v>
       </c>
@@ -14173,8 +15451,23 @@
       <c r="AQ84">
         <v>1</v>
       </c>
+      <c r="AR84">
+        <v>3.4228870007714102E-2</v>
+      </c>
+      <c r="AS84">
+        <v>5.6747444631806698E-2</v>
+      </c>
+      <c r="AT84">
+        <v>0.167098248494992</v>
+      </c>
+      <c r="AU84">
+        <v>5.1071616492417801E-2</v>
+      </c>
+      <c r="AV84" t="s">
+        <v>767</v>
+      </c>
     </row>
-    <row r="85" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>83</v>
       </c>
@@ -14304,8 +15597,23 @@
       <c r="AQ85">
         <v>1</v>
       </c>
+      <c r="AR85">
+        <v>0.29580802265957301</v>
+      </c>
+      <c r="AS85">
+        <v>0.28576289465232102</v>
+      </c>
+      <c r="AT85">
+        <v>0.322213258458517</v>
+      </c>
+      <c r="AU85">
+        <v>0.18048573635029</v>
+      </c>
+      <c r="AV85" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="86" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>84</v>
       </c>
@@ -14435,8 +15743,23 @@
       <c r="AQ86">
         <v>1</v>
       </c>
+      <c r="AR86">
+        <v>0.38221840022190601</v>
+      </c>
+      <c r="AS86">
+        <v>0.17915470912607501</v>
+      </c>
+      <c r="AT86">
+        <v>5.5105186947498601E-2</v>
+      </c>
+      <c r="AU86">
+        <v>9.7535399270617107E-2</v>
+      </c>
+      <c r="AV86" t="s">
+        <v>766</v>
+      </c>
     </row>
-    <row r="87" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>85</v>
       </c>
@@ -14566,8 +15889,23 @@
       <c r="AQ87">
         <v>1</v>
       </c>
+      <c r="AR87">
+        <v>1.9649069258256501E-2</v>
+      </c>
+      <c r="AS87">
+        <v>7.9786296373786994E-2</v>
+      </c>
+      <c r="AT87">
+        <v>0.217369418152452</v>
+      </c>
+      <c r="AU87">
+        <v>3.2432790130622703E-2</v>
+      </c>
+      <c r="AV87" t="s">
+        <v>767</v>
+      </c>
     </row>
-    <row r="88" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>86</v>
       </c>
@@ -14697,8 +16035,23 @@
       <c r="AQ88">
         <v>8.8110964683263807E-2</v>
       </c>
+      <c r="AR88">
+        <v>3.3535806629703298E-2</v>
+      </c>
+      <c r="AS88">
+        <v>0.132726455736841</v>
+      </c>
+      <c r="AT88">
+        <v>5.7284502761605599E-2</v>
+      </c>
+      <c r="AU88">
+        <v>1.1707811967664201E-2</v>
+      </c>
+      <c r="AV88" t="s">
+        <v>764</v>
+      </c>
     </row>
-    <row r="89" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>87</v>
       </c>
@@ -14828,8 +16181,23 @@
       <c r="AQ89" s="1">
         <v>6.9764843805621097E-5</v>
       </c>
+      <c r="AR89">
+        <v>0.24763360996150599</v>
+      </c>
+      <c r="AS89">
+        <v>0.16967093068265501</v>
+      </c>
+      <c r="AT89">
+        <v>9.6916792077621106E-2</v>
+      </c>
+      <c r="AU89">
+        <v>0.10598591727578301</v>
+      </c>
+      <c r="AV89" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="90" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>88</v>
       </c>
@@ -14959,8 +16327,23 @@
       <c r="AQ90">
         <v>1</v>
       </c>
+      <c r="AR90">
+        <v>0.166182611605936</v>
+      </c>
+      <c r="AS90">
+        <v>0.18139967642655899</v>
+      </c>
+      <c r="AT90">
+        <v>4.6886502848284398E-2</v>
+      </c>
+      <c r="AU90">
+        <v>6.3457907626463E-2</v>
+      </c>
+      <c r="AV90" t="s">
+        <v>768</v>
+      </c>
     </row>
-    <row r="91" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>89</v>
       </c>
@@ -15090,8 +16473,23 @@
       <c r="AQ91">
         <v>1</v>
       </c>
+      <c r="AR91">
+        <v>0.262674573072117</v>
+      </c>
+      <c r="AS91">
+        <v>6.4061365573942194E-2</v>
+      </c>
+      <c r="AT91">
+        <v>1.0193169502506099E-2</v>
+      </c>
+      <c r="AU91">
+        <v>7.34077974354818E-2</v>
+      </c>
+      <c r="AV91" t="s">
+        <v>766</v>
+      </c>
     </row>
-    <row r="92" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>90</v>
       </c>
@@ -15221,8 +16619,23 @@
       <c r="AQ92">
         <v>1</v>
       </c>
+      <c r="AR92">
+        <v>1.48081695720771E-2</v>
+      </c>
+      <c r="AS92">
+        <v>4.4723679692697797E-2</v>
+      </c>
+      <c r="AT92">
+        <v>0.12727436373547099</v>
+      </c>
+      <c r="AU92">
+        <v>9.0975251131272996E-3</v>
+      </c>
+      <c r="AV92" t="s">
+        <v>767</v>
+      </c>
     </row>
-    <row r="93" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>91</v>
       </c>
@@ -15352,8 +16765,23 @@
       <c r="AQ93">
         <v>1</v>
       </c>
+      <c r="AR93">
+        <v>0.36710569412349803</v>
+      </c>
+      <c r="AS93">
+        <v>0.234583503166892</v>
+      </c>
+      <c r="AT93">
+        <v>0.26253658896203302</v>
+      </c>
+      <c r="AU93">
+        <v>0.16575579696873999</v>
+      </c>
+      <c r="AV93" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="94" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>92</v>
       </c>
@@ -15483,8 +16911,23 @@
       <c r="AQ94">
         <v>1</v>
       </c>
+      <c r="AR94">
+        <v>0.34843759677928199</v>
+      </c>
+      <c r="AS94">
+        <v>0.13670138676129701</v>
+      </c>
+      <c r="AT94">
+        <v>3.72918494079734E-2</v>
+      </c>
+      <c r="AU94">
+        <v>0.102169260643659</v>
+      </c>
+      <c r="AV94" t="s">
+        <v>766</v>
+      </c>
     </row>
-    <row r="95" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>93</v>
       </c>
@@ -15614,8 +17057,23 @@
       <c r="AQ95">
         <v>1</v>
       </c>
+      <c r="AR95">
+        <v>5.153647668585E-2</v>
+      </c>
+      <c r="AS95">
+        <v>0.48299508452469297</v>
+      </c>
+      <c r="AT95">
+        <v>0.25424943538616701</v>
+      </c>
+      <c r="AU95">
+        <v>0.13338368097925801</v>
+      </c>
+      <c r="AV95" t="s">
+        <v>765</v>
+      </c>
     </row>
-    <row r="96" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>94</v>
       </c>
@@ -15745,8 +17203,23 @@
       <c r="AQ96">
         <v>1</v>
       </c>
+      <c r="AR96">
+        <v>6.9025630436642393E-2</v>
+      </c>
+      <c r="AS96">
+        <v>5.62469308217197E-2</v>
+      </c>
+      <c r="AT96">
+        <v>0.18120608337073599</v>
+      </c>
+      <c r="AU96">
+        <v>5.5648682688465803E-2</v>
+      </c>
+      <c r="AV96" t="s">
+        <v>767</v>
+      </c>
     </row>
-    <row r="97" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>95</v>
       </c>
@@ -15876,8 +17349,23 @@
       <c r="AQ97">
         <v>1</v>
       </c>
+      <c r="AR97">
+        <v>3.4628360437118401E-2</v>
+      </c>
+      <c r="AS97">
+        <v>5.1071018977830701E-2</v>
+      </c>
+      <c r="AT97">
+        <v>0.227014918883545</v>
+      </c>
+      <c r="AU97">
+        <v>2.93313319513713E-2</v>
+      </c>
+      <c r="AV97" t="s">
+        <v>767</v>
+      </c>
     </row>
-    <row r="98" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>96</v>
       </c>
@@ -16007,8 +17495,23 @@
       <c r="AQ98">
         <v>1</v>
       </c>
+      <c r="AR98">
+        <v>0.11623028447802999</v>
+      </c>
+      <c r="AS98">
+        <v>0.19251221958172901</v>
+      </c>
+      <c r="AT98">
+        <v>0.101641784321131</v>
+      </c>
+      <c r="AU98">
+        <v>8.3587140933692697E-2</v>
+      </c>
+      <c r="AV98" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="99" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>97</v>
       </c>
@@ -16138,8 +17641,23 @@
       <c r="AQ99">
         <v>1</v>
       </c>
+      <c r="AR99">
+        <v>0.10389471323231</v>
+      </c>
+      <c r="AS99">
+        <v>0.10780767189316</v>
+      </c>
+      <c r="AT99">
+        <v>5.8396497820150897E-2</v>
+      </c>
+      <c r="AU99">
+        <v>4.0871517004645398E-2</v>
+      </c>
+      <c r="AV99" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="100" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>98</v>
       </c>
@@ -16269,8 +17787,23 @@
       <c r="AQ100">
         <v>1</v>
       </c>
+      <c r="AR100">
+        <v>0.168417378499611</v>
+      </c>
+      <c r="AS100">
+        <v>0.220596822680375</v>
+      </c>
+      <c r="AT100">
+        <v>0.34881713830814798</v>
+      </c>
+      <c r="AU100">
+        <v>0.119637691225501</v>
+      </c>
+      <c r="AV100" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="101" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>99</v>
       </c>
@@ -16400,8 +17933,23 @@
       <c r="AQ101">
         <v>1</v>
       </c>
+      <c r="AR101">
+        <v>6.8010509514295797E-2</v>
+      </c>
+      <c r="AS101">
+        <v>9.7937928666221197E-2</v>
+      </c>
+      <c r="AT101">
+        <v>0.27616319735343198</v>
+      </c>
+      <c r="AU101">
+        <v>8.3176783990759895E-2</v>
+      </c>
+      <c r="AV101" t="s">
+        <v>767</v>
+      </c>
     </row>
-    <row r="102" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>100</v>
       </c>
@@ -16531,8 +18079,23 @@
       <c r="AQ102">
         <v>1</v>
       </c>
+      <c r="AR102">
+        <v>4.4663060017211903E-2</v>
+      </c>
+      <c r="AS102">
+        <v>0.13069514557324199</v>
+      </c>
+      <c r="AT102">
+        <v>0.192627226148222</v>
+      </c>
+      <c r="AU102">
+        <v>4.6344766647650103E-2</v>
+      </c>
+      <c r="AV102" t="s">
+        <v>767</v>
+      </c>
     </row>
-    <row r="103" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>101</v>
       </c>
@@ -16662,8 +18225,23 @@
       <c r="AQ103">
         <v>1</v>
       </c>
+      <c r="AR103">
+        <v>0.36163734582123103</v>
+      </c>
+      <c r="AS103">
+        <v>0.14071592248065701</v>
+      </c>
+      <c r="AT103">
+        <v>5.1399245015027101E-2</v>
+      </c>
+      <c r="AU103">
+        <v>9.0572324812866298E-2</v>
+      </c>
+      <c r="AV103" t="s">
+        <v>766</v>
+      </c>
     </row>
-    <row r="104" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>102</v>
       </c>
@@ -16793,8 +18371,23 @@
       <c r="AQ104">
         <v>1</v>
       </c>
+      <c r="AR104">
+        <v>0.111094181769095</v>
+      </c>
+      <c r="AS104">
+        <v>8.5692970171344696E-2</v>
+      </c>
+      <c r="AT104">
+        <v>0.37466147687576301</v>
+      </c>
+      <c r="AU104">
+        <v>0.10781378316586</v>
+      </c>
+      <c r="AV104" t="s">
+        <v>767</v>
+      </c>
     </row>
-    <row r="105" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>103</v>
       </c>
@@ -16924,8 +18517,23 @@
       <c r="AQ105">
         <v>1</v>
       </c>
+      <c r="AR105">
+        <v>-1.17711935912774E-2</v>
+      </c>
+      <c r="AS105">
+        <v>3.8051300928665E-3</v>
+      </c>
+      <c r="AT105">
+        <v>0.42137823431745702</v>
+      </c>
+      <c r="AU105">
+        <v>-2.6217859603379001E-3</v>
+      </c>
+      <c r="AV105" t="s">
+        <v>767</v>
+      </c>
     </row>
-    <row r="106" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>104</v>
       </c>
@@ -17055,8 +18663,23 @@
       <c r="AQ106">
         <v>1</v>
       </c>
+      <c r="AR106">
+        <v>0.48414901971790902</v>
+      </c>
+      <c r="AS106">
+        <v>0.18668107351959901</v>
+      </c>
+      <c r="AT106">
+        <v>3.7648907670759797E-2</v>
+      </c>
+      <c r="AU106">
+        <v>7.2489908369905307E-2</v>
+      </c>
+      <c r="AV106" t="s">
+        <v>766</v>
+      </c>
     </row>
-    <row r="107" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>105</v>
       </c>
@@ -17186,8 +18809,23 @@
       <c r="AQ107">
         <v>1</v>
       </c>
+      <c r="AR107">
+        <v>0.36295124321286998</v>
+      </c>
+      <c r="AS107">
+        <v>9.8820120714134305E-2</v>
+      </c>
+      <c r="AT107">
+        <v>2.1683013812557401E-2</v>
+      </c>
+      <c r="AU107">
+        <v>5.8439687501210598E-2</v>
+      </c>
+      <c r="AV107" t="s">
+        <v>766</v>
+      </c>
     </row>
-    <row r="108" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>106</v>
       </c>
@@ -17317,8 +18955,23 @@
       <c r="AQ108">
         <v>1</v>
       </c>
+      <c r="AR108">
+        <v>0.28307013297014499</v>
+      </c>
+      <c r="AS108">
+        <v>7.9958533610863206E-2</v>
+      </c>
+      <c r="AT108">
+        <v>6.0316869610292E-2</v>
+      </c>
+      <c r="AU108">
+        <v>6.9853487169400097E-2</v>
+      </c>
+      <c r="AV108" t="s">
+        <v>766</v>
+      </c>
     </row>
-    <row r="109" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>107</v>
       </c>
@@ -17448,8 +19101,23 @@
       <c r="AQ109">
         <v>1</v>
       </c>
+      <c r="AR109">
+        <v>7.4705122379974703E-2</v>
+      </c>
+      <c r="AS109">
+        <v>7.0581344667149298E-2</v>
+      </c>
+      <c r="AT109">
+        <v>0.35315478797448602</v>
+      </c>
+      <c r="AU109">
+        <v>0.100313280243879</v>
+      </c>
+      <c r="AV109" t="s">
+        <v>767</v>
+      </c>
     </row>
-    <row r="110" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>108</v>
       </c>
@@ -17579,8 +19247,23 @@
       <c r="AQ110">
         <v>2.3794824504739701E-4</v>
       </c>
+      <c r="AR110">
+        <v>0.34363766792706701</v>
+      </c>
+      <c r="AS110">
+        <v>0.24107893908767</v>
+      </c>
+      <c r="AT110">
+        <v>0.38816597650156698</v>
+      </c>
+      <c r="AU110">
+        <v>0.15852204065464601</v>
+      </c>
+      <c r="AV110" t="s">
+        <v>763</v>
+      </c>
     </row>
-    <row r="111" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>109</v>
       </c>
@@ -17710,8 +19393,23 @@
       <c r="AQ111">
         <v>1</v>
       </c>
+      <c r="AR111">
+        <v>3.9248112075492801E-2</v>
+      </c>
+      <c r="AS111">
+        <v>5.3211923173604299E-2</v>
+      </c>
+      <c r="AT111">
+        <v>0.29121290438076097</v>
+      </c>
+      <c r="AU111">
+        <v>5.2853807980403497E-2</v>
+      </c>
+      <c r="AV111" t="s">
+        <v>767</v>
+      </c>
     </row>
-    <row r="112" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>110</v>
       </c>
@@ -17841,8 +19539,23 @@
       <c r="AQ112">
         <v>1</v>
       </c>
+      <c r="AR112">
+        <v>5.73771025867248E-2</v>
+      </c>
+      <c r="AS112">
+        <v>5.5012014814709298E-2</v>
+      </c>
+      <c r="AT112">
+        <v>0.25209150350947102</v>
+      </c>
+      <c r="AU112">
+        <v>5.7645210367781502E-2</v>
+      </c>
+      <c r="AV112" t="s">
+        <v>767</v>
+      </c>
     </row>
-    <row r="113" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>111</v>
       </c>
@@ -17971,6 +19684,21 @@
       </c>
       <c r="AQ113">
         <v>6.5804355447058899E-2</v>
+      </c>
+      <c r="AR113">
+        <v>0.18500936463165399</v>
+      </c>
+      <c r="AS113">
+        <v>0.156122485146936</v>
+      </c>
+      <c r="AT113">
+        <v>0.381914944126369</v>
+      </c>
+      <c r="AU113">
+        <v>8.8984295372876193E-2</v>
+      </c>
+      <c r="AV113" t="s">
+        <v>767</v>
       </c>
     </row>
   </sheetData>

</xml_diff>